<commit_message>
impledted new pages and test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Swag_lab_data.xlsx
+++ b/src/test/resources/excel/Swag_lab_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul Kashyap\PracticeAllConcepts\OpenCart_POM\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3788A5F5-2687-43AA-8849-F1A06F1620DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E29AB8F-245B-45B0-AEB1-274801799371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginTest" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,10 @@
     <sheet name="verifyCartBadgeAndCartItemMatch" sheetId="13" r:id="rId10"/>
     <sheet name="verfiyFormDetails" sheetId="14" r:id="rId11"/>
     <sheet name="verifyCancelBtn" sheetId="15" r:id="rId12"/>
-    <sheet name="invalidLoginTest" sheetId="2" r:id="rId13"/>
-    <sheet name="lockedOutUserTest" sheetId="3" r:id="rId14"/>
+    <sheet name="verifycheckoutOverview" sheetId="16" r:id="rId13"/>
+    <sheet name="verifyFinishCheckout" sheetId="17" r:id="rId14"/>
+    <sheet name="invalidLoginTest" sheetId="2" r:id="rId15"/>
+    <sheet name="lockedOutUserTest" sheetId="3" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t>password</t>
   </si>
@@ -191,6 +193,9 @@
   </si>
   <si>
     <t>Overview page not displayed</t>
+  </si>
+  <si>
+    <t>R42201</t>
   </si>
 </sst>
 </file>
@@ -652,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD6019A-FA1F-4C5B-876D-0700F253FCAE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -678,6 +683,104 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CD4385-32A0-4A77-A5CF-887E1703E127}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE1C58A-17C4-41DB-97A1-25EEEA45B741}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5691473-0634-4B3F-B05F-56C8B4C17074}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -714,7 +817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFF7F3F-A69E-42A1-9B72-36BD2F0F28D9}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>